<commit_message>
Added weight field to the HS-Cooler calculator
</commit_message>
<xml_diff>
--- a/acc_main/data/hs_prices.xlsx
+++ b/acc_main/data/hs_prices.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubenhias/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubenhias/PycharmProjects/odoo/atlantic/acc_main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CE00DD-713E-CD4D-AF9A-79B981B0388D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E639BD-B5F1-E846-B8F1-836A7DF8CB62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{B5D00337-6CD4-4F40-BA06-0A95214C57CD}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="15960" xr2:uid="{B5D00337-6CD4-4F40-BA06-0A95214C57CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Pattern</t>
   </si>
@@ -159,16 +159,29 @@
   </si>
   <si>
     <t>KS25P</t>
+  </si>
+  <si>
+    <t>Baseweight</t>
+  </si>
+  <si>
+    <t>Lengthweight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,8 +207,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,18 +524,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA70784-12DF-4D4D-81C1-2340D4D1E5E2}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,8 +546,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -542,8 +563,14 @@
       <c r="C2">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>5.9</v>
+      </c>
+      <c r="E2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -553,8 +580,14 @@
       <c r="C3">
         <v>43.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>23.9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.24545500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -564,8 +597,14 @@
       <c r="C4">
         <v>38.700000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>23.9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.22272700000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -575,8 +614,14 @@
       <c r="C5">
         <v>35.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>23.9</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.21363599999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -586,8 +631,14 @@
       <c r="C6">
         <v>43.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>26.9</v>
+      </c>
+      <c r="E6">
+        <v>0.24545454545454543</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -597,8 +648,14 @@
       <c r="C7">
         <v>38.700000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>26.9</v>
+      </c>
+      <c r="E7">
+        <v>0.22272727272727275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -608,8 +665,14 @@
       <c r="C8">
         <v>35.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>26.9</v>
+      </c>
+      <c r="E8">
+        <v>0.21363636363636362</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -619,8 +682,14 @@
       <c r="C9">
         <v>43.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>31.9</v>
+      </c>
+      <c r="E9">
+        <v>0.24545454545454543</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -630,8 +699,14 @@
       <c r="C10">
         <v>38.700000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>31.9</v>
+      </c>
+      <c r="E10">
+        <v>0.22272727272727275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -641,8 +716,14 @@
       <c r="C11">
         <v>35.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>31.9</v>
+      </c>
+      <c r="E11">
+        <v>0.21363636363636362</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -652,8 +733,14 @@
       <c r="C12">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>60.4</v>
+      </c>
+      <c r="E12">
+        <v>0.58181818181818179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -663,8 +750,14 @@
       <c r="C13">
         <v>80.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>60.4</v>
+      </c>
+      <c r="E13">
+        <v>0.53181818181818186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -674,8 +767,14 @@
       <c r="C14">
         <v>73.2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>60.4</v>
+      </c>
+      <c r="E14">
+        <v>0.50454545454545452</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -685,8 +784,14 @@
       <c r="C15">
         <v>92</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>61.4</v>
+      </c>
+      <c r="E15">
+        <v>0.58181818181818179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -696,8 +801,14 @@
       <c r="C16">
         <v>80.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>61.4</v>
+      </c>
+      <c r="E16">
+        <v>0.53181818181818186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -707,8 +818,14 @@
       <c r="C17">
         <v>73.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>61.4</v>
+      </c>
+      <c r="E17">
+        <v>0.50454545454545452</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -718,8 +835,14 @@
       <c r="C18">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E18">
+        <v>0.58181818181818179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -729,8 +852,14 @@
       <c r="C19">
         <v>80.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E19">
+        <v>0.53181818181818186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -740,8 +869,14 @@
       <c r="C20">
         <v>73.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E20">
+        <v>0.50454545454545452</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -751,8 +886,14 @@
       <c r="C21">
         <v>130.69999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>106.7</v>
+      </c>
+      <c r="E21">
+        <v>0.80909090909090908</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -762,8 +903,14 @@
       <c r="C22">
         <v>116</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>106.7</v>
+      </c>
+      <c r="E22">
+        <v>0.74090909090909096</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -773,8 +920,14 @@
       <c r="C23">
         <v>107.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>106.7</v>
+      </c>
+      <c r="E23">
+        <v>0.70000000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -784,8 +937,14 @@
       <c r="C24">
         <v>130.69999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>109.7</v>
+      </c>
+      <c r="E24">
+        <v>0.80909090909090908</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -795,8 +954,14 @@
       <c r="C25">
         <v>116</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>109.7</v>
+      </c>
+      <c r="E25">
+        <v>0.74090909090909096</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -806,8 +971,14 @@
       <c r="C26">
         <v>107.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>109.7</v>
+      </c>
+      <c r="E26">
+        <v>0.70000000000000007</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -817,8 +988,14 @@
       <c r="C27">
         <v>130.69999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>179.7</v>
+      </c>
+      <c r="E27">
+        <v>0.80909090909090908</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -828,8 +1005,14 @@
       <c r="C28">
         <v>116</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>179.7</v>
+      </c>
+      <c r="E28">
+        <v>0.74090909090909096</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -839,8 +1022,14 @@
       <c r="C29">
         <v>107.7</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>179.7</v>
+      </c>
+      <c r="E29">
+        <v>0.70000000000000007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -850,8 +1039,14 @@
       <c r="C30">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -861,8 +1056,14 @@
       <c r="C31">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -872,8 +1073,14 @@
       <c r="C32">
         <v>16.8</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -883,8 +1090,14 @@
       <c r="C33">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -892,7 +1105,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -900,7 +1113,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -908,7 +1121,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -916,28 +1129,37 @@
         <v>544</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38">
         <v>300</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
       <c r="B39">
         <v>480</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
       <c r="B40">
         <v>600</v>
+      </c>
+      <c r="D40">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>